<commit_message>
Fixing the error in venue splitting
</commit_message>
<xml_diff>
--- a/finalData.xlsx
+++ b/finalData.xlsx
@@ -5336,7 +5336,7 @@
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -5405,7 +5405,7 @@
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>
@@ -15686,7 +15686,7 @@
       </c>
       <c r="O222" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -15755,7 +15755,7 @@
       </c>
       <c r="O223" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>
@@ -25070,7 +25070,7 @@
       </c>
       <c r="O358" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -25139,7 +25139,7 @@
       </c>
       <c r="O359" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>
@@ -26450,7 +26450,7 @@
       </c>
       <c r="O378" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -26519,7 +26519,7 @@
       </c>
       <c r="O379" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>
@@ -34799,7 +34799,7 @@
       </c>
       <c r="O499" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -34868,7 +34868,7 @@
       </c>
       <c r="O500" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>
@@ -35972,7 +35972,7 @@
       </c>
       <c r="O516" t="inlineStr">
         <is>
-          <t xml:space="preserve">NFC III </t>
+          <t>NFC III</t>
         </is>
       </c>
     </row>
@@ -36041,7 +36041,7 @@
       </c>
       <c r="O517" t="inlineStr">
         <is>
-          <t>NFC III  NFC IV</t>
+          <t>NFC IV</t>
         </is>
       </c>
     </row>

</xml_diff>